<commit_message>
Added styling to cell in output
</commit_message>
<xml_diff>
--- a/ExcelExports/temp.xlsx
+++ b/ExcelExports/temp.xlsx
@@ -114,13 +114,43 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,8 +173,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -158,43 +194,43 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s" s="1">
         <v>6</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s" s="1">
         <v>11</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="1">
         <v>13</v>
       </c>
     </row>
@@ -786,46 +822,46 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="S1" t="s" s="0">
+      <c r="S1" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
+      <c r="V1" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="Y1" t="s" s="0">
+      <c r="Y1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="AB1" t="s" s="0">
+      <c r="AB1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="AE1" t="s" s="0">
+      <c r="AE1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="AH1" t="s" s="0">
+      <c r="AH1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="AK1" t="s" s="0">
+      <c r="AK1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="AN1" t="s" s="0">
+      <c r="AN1" t="s" s="2">
         <v>27</v>
       </c>
     </row>
@@ -1015,46 +1051,46 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="3">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="3">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="S1" t="s" s="0">
+      <c r="S1" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
+      <c r="V1" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="Y1" t="s" s="0">
+      <c r="Y1" t="s" s="3">
         <v>22</v>
       </c>
-      <c r="AB1" t="s" s="0">
+      <c r="AB1" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="AE1" t="s" s="0">
+      <c r="AE1" t="s" s="3">
         <v>24</v>
       </c>
-      <c r="AH1" t="s" s="0">
+      <c r="AH1" t="s" s="3">
         <v>25</v>
       </c>
-      <c r="AK1" t="s" s="0">
+      <c r="AK1" t="s" s="3">
         <v>26</v>
       </c>
-      <c r="AN1" t="s" s="0">
+      <c r="AN1" t="s" s="3">
         <v>27</v>
       </c>
     </row>
@@ -1244,46 +1280,46 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="4">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s" s="4">
         <v>19</v>
       </c>
-      <c r="S1" t="s" s="0">
+      <c r="S1" t="s" s="4">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
+      <c r="V1" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="Y1" t="s" s="0">
+      <c r="Y1" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="AB1" t="s" s="0">
+      <c r="AB1" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="AE1" t="s" s="0">
+      <c r="AE1" t="s" s="4">
         <v>24</v>
       </c>
-      <c r="AH1" t="s" s="0">
+      <c r="AH1" t="s" s="4">
         <v>25</v>
       </c>
-      <c r="AK1" t="s" s="0">
+      <c r="AK1" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="AN1" t="s" s="0">
+      <c r="AN1" t="s" s="4">
         <v>27</v>
       </c>
     </row>
@@ -1473,46 +1509,46 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="S1" t="s" s="0">
+      <c r="S1" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
+      <c r="V1" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="Y1" t="s" s="0">
+      <c r="Y1" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="AB1" t="s" s="0">
+      <c r="AB1" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="AE1" t="s" s="0">
+      <c r="AE1" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="AH1" t="s" s="0">
+      <c r="AH1" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="AK1" t="s" s="0">
+      <c r="AK1" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="AN1" t="s" s="0">
+      <c r="AN1" t="s" s="5">
         <v>27</v>
       </c>
     </row>
@@ -1702,46 +1738,46 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s" s="6">
         <v>19</v>
       </c>
-      <c r="S1" t="s" s="0">
+      <c r="S1" t="s" s="6">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
+      <c r="V1" t="s" s="6">
         <v>21</v>
       </c>
-      <c r="Y1" t="s" s="0">
+      <c r="Y1" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="AB1" t="s" s="0">
+      <c r="AB1" t="s" s="6">
         <v>23</v>
       </c>
-      <c r="AE1" t="s" s="0">
+      <c r="AE1" t="s" s="6">
         <v>24</v>
       </c>
-      <c r="AH1" t="s" s="0">
+      <c r="AH1" t="s" s="6">
         <v>25</v>
       </c>
-      <c r="AK1" t="s" s="0">
+      <c r="AK1" t="s" s="6">
         <v>26</v>
       </c>
-      <c r="AN1" t="s" s="0">
+      <c r="AN1" t="s" s="6">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prepped for revamp of simulated stock
</commit_message>
<xml_diff>
--- a/ExcelExports/temp.xlsx
+++ b/ExcelExports/temp.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
   <si>
     <t/>
   </si>
@@ -103,13 +103,10 @@
     <t>Month: 13</t>
   </si>
   <si>
-    <t>Coupon Yield</t>
-  </si>
-  <si>
-    <t>Sale at Maturity</t>
-  </si>
-  <si>
-    <t>Maturity</t>
+    <t>Dividends</t>
+  </si>
+  <si>
+    <t>Capital Appreciation</t>
   </si>
 </sst>
 </file>
@@ -254,7 +251,7 @@
         <v>0.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G2" t="n" s="0">
         <v>0.0</v>
@@ -263,19 +260,19 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="K2" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.8409443766154858</v>
       </c>
     </row>
     <row r="3">
@@ -295,7 +292,7 @@
         <v>0.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="n" s="0">
         <v>0.0</v>
@@ -304,19 +301,19 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>5.0</v>
+        <v>12.0</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>5.0</v>
+        <v>12.0</v>
       </c>
       <c r="K3" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M3" t="n" s="0">
-        <v>0.0</v>
+        <v>1.6130352902246758</v>
       </c>
     </row>
     <row r="4">
@@ -336,7 +333,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="n" s="0">
         <v>0.0</v>
@@ -345,19 +342,19 @@
         <v>0.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>5.0</v>
+        <v>13.0</v>
       </c>
       <c r="K4" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L4" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M4" t="n" s="0">
-        <v>0.0</v>
+        <v>1.4334151101796073</v>
       </c>
     </row>
     <row r="5">
@@ -377,7 +374,7 @@
         <v>0.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="n" s="0">
         <v>0.0</v>
@@ -386,19 +383,19 @@
         <v>0.0</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="K5" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M5" t="n" s="0">
-        <v>0.0</v>
+        <v>1.2885409112665345</v>
       </c>
     </row>
     <row r="6">
@@ -418,7 +415,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" t="n" s="0">
         <v>0.0</v>
@@ -427,19 +424,19 @@
         <v>0.0</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="K6" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L6" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M6" t="n" s="0">
-        <v>0.0</v>
+        <v>1.1694252129716127</v>
       </c>
     </row>
     <row r="7">
@@ -459,7 +456,7 @@
         <v>0.0</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="n" s="0">
         <v>0.0</v>
@@ -468,19 +465,19 @@
         <v>0.0</v>
       </c>
       <c r="I7" t="n" s="0">
-        <v>5.0</v>
+        <v>16.0</v>
       </c>
       <c r="J7" t="n" s="0">
-        <v>5.0</v>
+        <v>16.0</v>
       </c>
       <c r="K7" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L7" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M7" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0698899917795224</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +497,7 @@
         <v>0.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>0.0</v>
@@ -509,19 +506,19 @@
         <v>0.0</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>5.0</v>
+        <v>17.0</v>
       </c>
       <c r="J8" t="n" s="0">
-        <v>5.0</v>
+        <v>17.0</v>
       </c>
       <c r="K8" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L8" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M8" t="n" s="0">
-        <v>0.0</v>
+        <v>0.9855599520654272</v>
       </c>
     </row>
     <row r="9">
@@ -541,7 +538,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G9" t="n" s="0">
         <v>0.0</v>
@@ -550,19 +547,19 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c r="K9" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L9" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M9" t="n" s="0">
-        <v>0.0</v>
+        <v>0.9132562918007303</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +579,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="n" s="0">
         <v>0.0</v>
@@ -591,19 +588,19 @@
         <v>0.0</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
       <c r="J10" t="n" s="0">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
       <c r="K10" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L10" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M10" t="n" s="0">
-        <v>0.0</v>
+        <v>0.8506178062217085</v>
       </c>
     </row>
     <row r="11">
@@ -623,7 +620,7 @@
         <v>0.0</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G11" t="n" s="0">
         <v>0.0</v>
@@ -632,19 +629,19 @@
         <v>0.0</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>5.0</v>
+        <v>20.0</v>
       </c>
       <c r="J11" t="n" s="0">
-        <v>5.0</v>
+        <v>20.0</v>
       </c>
       <c r="K11" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L11" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M11" t="n" s="0">
-        <v>0.0</v>
+        <v>0.7958563260221301</v>
       </c>
     </row>
     <row r="12">
@@ -664,7 +661,7 @@
         <v>0.0</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" t="n" s="0">
         <v>0.0</v>
@@ -673,19 +670,19 @@
         <v>0.0</v>
       </c>
       <c r="I12" t="n" s="0">
-        <v>5.0</v>
+        <v>21.0</v>
       </c>
       <c r="J12" t="n" s="0">
-        <v>5.0</v>
+        <v>21.0</v>
       </c>
       <c r="K12" t="n" s="0">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="L12" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M12" t="n" s="0">
-        <v>0.0</v>
+        <v>0.7475943544285117</v>
       </c>
     </row>
     <row r="13">
@@ -702,31 +699,31 @@
         <v>0.0</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>-10.0</v>
+        <v>0.0</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="I13" t="n" s="0">
-        <v>0.0</v>
+        <v>22.0</v>
       </c>
       <c r="J13" t="n" s="0">
-        <v>0.0</v>
+        <v>22.0</v>
       </c>
       <c r="K13" t="n" s="0">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="L13" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="M13" t="n" s="0">
-        <v>1.7976931348623157E308</v>
+        <v>0.7047545660620107</v>
       </c>
     </row>
     <row r="14">
@@ -746,7 +743,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="n" s="0">
         <v>0.0</v>
@@ -755,19 +752,19 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="J14" t="n" s="0">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="K14" t="n" s="0">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="L14" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M14" t="n" s="0">
-        <v>1.7976931348623157E308</v>
+        <v>0.6664829255615827</v>
       </c>
     </row>
     <row r="15">
@@ -787,7 +784,7 @@
         <v>0.0</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" t="n" s="0">
         <v>0.0</v>
@@ -796,19 +793,19 @@
         <v>0.0</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="J15" t="n" s="0">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="K15" t="n" s="0">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="L15" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M15" t="n" s="0">
-        <v>1.7976931348623157E308</v>
+        <v>0.6320941327229255</v>
       </c>
     </row>
   </sheetData>
@@ -869,10 +866,22 @@
       </c>
     </row>
     <row r="2">
+      <c r="G2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>0.0</v>
+      </c>
       <c r="P2" t="s" s="0">
         <v>28</v>
       </c>
       <c r="Q2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="AH2" t="s" s="0">
@@ -1003,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AN1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1053,14 +1062,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2">
-      <c r="AH2" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="AI2" t="n" s="0">
-        <v>-10.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1068,7 +1069,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1119,11 +1120,89 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="H2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="N2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="T2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="W2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AB2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AC2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AE2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AF2" t="n" s="0">
+        <v>1.0</v>
+      </c>
       <c r="AH2" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI2" t="n" s="0">
-        <v>5.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="AK2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AL2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="AN2" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="AO2" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>